<commit_message>
udate for release 2 - version 1
</commit_message>
<xml_diff>
--- a/TemplateMetadata.xlsx
+++ b/TemplateMetadata.xlsx
@@ -1,13 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E26A79-080D-4E94-9935-C972BFE21439}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23805" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="List1" sheetId="1" r:id="rId1"/>
+    <sheet name="samples" sheetId="1" r:id="rId1"/>
+    <sheet name="metadata_fields_description" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="132">
   <si>
     <t>Longitude</t>
   </si>
@@ -163,13 +165,265 @@
   </si>
   <si>
     <t>One of the following: aquatic/desert/grassland/forest/tundra/cropland/wetland/woodland/shrubland/mangrove/anthropogenic</t>
+  </si>
+  <si>
+    <t>VARIABLE</t>
+  </si>
+  <si>
+    <t>OPTIONS</t>
+  </si>
+  <si>
+    <t>HINTS</t>
+  </si>
+  <si>
+    <t>Geographical longitude where the sample has been collected, in decimal degrees and using the WGS 84 geodetic system (i.e., following the format: “56.789” if East or “-56.789” if West. If necessary, you can convert 'degrees, minutes, seconds' in 'decimal degrees' with https://www.gps-coordinates.net/).</t>
+  </si>
+  <si>
+    <t>Geographical latitude where the sample has been collected, in decimal degrees and using the WGS 84 geodetic system (i.e., following the format: “12.345” if North or “-12.345” if South. If necessary, you can convert 'degrees, minutes, seconds' in 'decimal degrees' with https://www.gps-coordinates.net/).</t>
+  </si>
+  <si>
+    <t>Elevation in meter above sea level.</t>
+  </si>
+  <si>
+    <t>One of the following:</t>
+  </si>
+  <si>
+    <t>Africa</t>
+  </si>
+  <si>
+    <t>Antarctica</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>North America</t>
+  </si>
+  <si>
+    <t>South America</t>
+  </si>
+  <si>
+    <t>Specify the continent where the sample has been collected.</t>
+  </si>
+  <si>
+    <t>Country where the sample has been collected.</t>
+  </si>
+  <si>
+    <t>Geographic location where the sample has been collected, in geographic terms, not sample Ids. (example: “Tajen Forest Station, southeastern Taiwan” or “Deschutes National Forest, Oregon, USA”).</t>
+  </si>
+  <si>
+    <t>soil</t>
+  </si>
+  <si>
+    <t>rhizosphere soil</t>
+  </si>
+  <si>
+    <t>litter</t>
+  </si>
+  <si>
+    <t>topsoil</t>
+  </si>
+  <si>
+    <t>deadwood</t>
+  </si>
+  <si>
+    <t>lichen</t>
+  </si>
+  <si>
+    <t>shoot</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>air</t>
+  </si>
+  <si>
+    <t>dust</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>sediment</t>
+  </si>
+  <si>
+    <t>Specify the type of sample collected. Note that “soil” includes the samples belonging to all the soil layers, i.e., organic horizon or humus, mineral horizon, subsoil, substratum or parent rock, bedrock. “shoot” includes all the part (living or dead) of the plant that are aboveground (example: leaf, fruit, branch, stem, …), except for deadwood, litter and lichen for which you can write “deadwood”, “litter” and “lichen”, respectively. “topsoil” includes a mix of litter and soil, whatever the depth of soil collected.</t>
+  </si>
+  <si>
+    <t>aquatic</t>
+  </si>
+  <si>
+    <t>desert</t>
+  </si>
+  <si>
+    <t>grassland</t>
+  </si>
+  <si>
+    <t>forest</t>
+  </si>
+  <si>
+    <t>tundra</t>
+  </si>
+  <si>
+    <t>cropland</t>
+  </si>
+  <si>
+    <t>wetland</t>
+  </si>
+  <si>
+    <t>woodland</t>
+  </si>
+  <si>
+    <t>shrubland</t>
+  </si>
+  <si>
+    <t>mangrove</t>
+  </si>
+  <si>
+    <t>anthropogenic</t>
+  </si>
+  <si>
+    <t>Select the environment where the sample has been collected among the proposed list.</t>
+  </si>
+  <si>
+    <t>Specify here the ecosystem/biome where the sample has been collected as specifically as possible among the ecosystem/biome classification located at http://www.ontobee.org/ontology/catalog/ENVO?iri=http://purl.obolibrary.org/obo/ENVO_01001110 and http://www.ontobee.org/ontology/ENVO?iri=http://purl.obolibrary.org/obo/ENVO_00000446. When you click on one term, you will get a list of more specific terms; By clicking on the appropriate term, you can move to more and more specific descriptions of the sampled ecosystem/biome. Continue to select the options as long as you are SURE that the sample fits. When you are unable to decide, use just a general term (example: “forest ecosystem” instead of “broadleaf forest biome”).</t>
+  </si>
+  <si>
+    <t>Mean annual temperature in degrees Celsius.</t>
+  </si>
+  <si>
+    <t>Mean annual precipitation in mm.</t>
+  </si>
+  <si>
+    <t>The name that you choose to give to the sample or the sample name provided in the manuscript. Examples: “USA_soil_1”, “Forest_1”, “Forest_2”, “AK1”, …</t>
+  </si>
+  <si>
+    <t>Area, in square meters, covered by sampling if multiple subsamples were collected, for single subsample = 1.</t>
+  </si>
+  <si>
+    <t>Estimate of area size in square meters, if exact location is not available.</t>
+  </si>
+  <si>
+    <t>How many subsamples were collected and combined within the area sampled to make up a sample for DNA extraction.</t>
+  </si>
+  <si>
+    <t>Depth of sampling, in cm, for soil/sediment/litter. Examples: “0 to 10” , “15 to 25”,…</t>
+  </si>
+  <si>
+    <t>Specify the year of sample collection.</t>
+  </si>
+  <si>
+    <t>Specify the month of sample collection.</t>
+  </si>
+  <si>
+    <t>Specify the day of sample collection.</t>
+  </si>
+  <si>
+    <t>Additional information specifying sampling design. For soil cores, specify the core diameter, in cm, or corresponding value. For roots, specify the sampled length and/or mass. For deadwood, specify the sampled volume (including unit of measurement). Etc.</t>
+  </si>
+  <si>
+    <t>Additional information specifying sample type. - If sample type is “soil”, please specify the soil layer if possible (i.e., “organic horizon=humus”&gt; “mineral horizon”&gt; “subsoil”&gt; “substratum=parent rock”&gt; “bedrock”). - If sample type is some plant material: specify what exactly the sample is. Examples: “deadwood, heartwood of several branches” or “lichens, whole plant”; or specify what part of the plant: “leaf, several randomly selected needles”, “fruit, several grape berries”, “petiole”, “root endosphere”, “seed”, “roots, ectomycorrhizae (ECM) root tips”, …</t>
+  </si>
+  <si>
+    <t>Illumina</t>
+  </si>
+  <si>
+    <t>454Roche</t>
+  </si>
+  <si>
+    <t>PacBio</t>
+  </si>
+  <si>
+    <t>IonTorrent</t>
+  </si>
+  <si>
+    <t>SOLiD</t>
+  </si>
+  <si>
+    <t>Oxford Nanopore</t>
+  </si>
+  <si>
+    <t>Specify the platform used for the sequencing of the sample.</t>
+  </si>
+  <si>
+    <t>ITS1</t>
+  </si>
+  <si>
+    <t>ITS2</t>
+  </si>
+  <si>
+    <t>ITSboth</t>
+  </si>
+  <si>
+    <t>Specify the molecular marker that you analyzed. Note that ITSboth = both ITS1 and ITS2.</t>
+  </si>
+  <si>
+    <t>Total mass of the sample used for DNA extraction in grams of material (Note that if, for example, the DNA extraction has been made in triplicate with 0.2 g each: please write the total mass used, i.e., 0.6)</t>
+  </si>
+  <si>
+    <t>If the total mass of the sample used for DNA extraction is not available, specify here the other definition of size of sample used for DNA extraction.</t>
+  </si>
+  <si>
+    <t>Please specify the method/kit used for DNA extraction from the sample.</t>
+  </si>
+  <si>
+    <t>Specify the name of the primers used. Example: “ITS1F/ITS2”.</t>
+  </si>
+  <si>
+    <t>Specify the sequences of each primers used. Example: “CTTGGTCATTTAGAGGAAGTAA/GCTGCGTTCTTCATCGATGC”.</t>
+  </si>
+  <si>
+    <t>Indicate the pH of the sample.</t>
+  </si>
+  <si>
+    <t>Indicate the pH measurement method: “H2O” or “KOH” or “KCl” or “CaCl2” or “other extract”.</t>
+  </si>
+  <si>
+    <t>Content of organic matter in % in your sample (Note that 1 g.kg-1 = 1 mg.g-1 = 1x10-1 % and 1 mg.kg-1 = 1 μg.g-1 = 1x10-4 %) (If the unit is different, please specify the unit in parentheses, after the value).</t>
+  </si>
+  <si>
+    <t>Content of organic Carbon in % in your sample (Note that 1 g.kg-1 = 1 mg.g-1 = 1x10-1 % and 1 mg.kg-1 = 1 μg.g-1 = 1x10-4 %) (If the unit is different, please specify the unit in parentheses, after the value).</t>
+  </si>
+  <si>
+    <t>Total Nitrogen content in % in your sample (Note that 1 g.kg-1 = 1 mg.g-1 = 1x10-1 % and 1 mg.kg-1 = 1 μg.g-1 = 1x10-4 %) (If the unit is different, please specify the unit in parentheses, after the value).</t>
+  </si>
+  <si>
+    <t>Total Phosphorus content in ppm in your sample (Note that 1 ppm = 1 mg.kg-1 = 1 μg.g-1 = 0.001 g.kg-1) (If the unit is different, please specify the unit in parentheses, after the value)</t>
+  </si>
+  <si>
+    <t>Total Calcium content in ppm in your sample (Note that 1 ppm = 1 mg.kg-1 = 1 μg.g-1 = 0.001 g.kg-1) (If the unit is different, please specify the unit in parentheses, after the value)</t>
+  </si>
+  <si>
+    <t>Total Potassium content in ppm in your sample (Note that 1 ppm = 1 mg.kg-1 = 1 μg.g-1 = 0.001 g.kg-1) (If the unit is different, please specify the unit in parentheses, after the value)</t>
+  </si>
+  <si>
+    <t>Please use the Latin names of the dominant primary producer(s) at the sampling site (example: replace Norway spruce with Picea abies). For plant material, specify the plant species to which the sample belongs.</t>
+  </si>
+  <si>
+    <t>Please use the Latin names of the other plants present at the sampling site (example: replace Norway spruce with Picea abies) or the most precise classification that you can give (e.g., genus). Should be only those plants not listed in the Dominant plant(s) species. - For a litter sample, if you know all the plant species that compose the litter please specify all the species (example: “species 1, species 2, species 3”). - For a soil sample, specify the surrounding tree(s) and/or vegetation if possible (example: “species 1, species 2, species 3”).</t>
+  </si>
+  <si>
+    <t>Additional information available for the sample including additional metadata (such as other chemical, physical or biological properties of the sample/location, ….)</t>
+  </si>
+  <si>
+    <t>Identifier of the raw sequencing data corresponding to the sample. - If the raw sequences of the sample are under Fastq or Fasta format in a public repository: provide the accession number allowing to download the Fastq/Fasta file of the sample (examples: “SRR25497”, “ERR25498”, “DRR25489”,…). - If the raw sequences of the sample are under Fastq or Fasta format NOT in a public repository: provide the name of the Fastq/Fasta file corresponding to the sample (example: “SampleName.fastq”). - If the raw sequences of the sample are merged with the raw sequences of other samples: provide the link to the sequencing data here and specify in the “Sample barcode/identifier” column the barcode sequence corresponding to the sample and allowing to differentiate it from the other samples. Note that each sample MUST HAVE a unique sequence identifier and/or a unique barcode/identifier allowing to identify it unambiguously!</t>
+  </si>
+  <si>
+    <t>If the raw sequences of the sample are merged with the sequences of other samples, provide the barcode sequence or identifier corresponding to the sample and allowing to differentiate it from the others.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,6 +450,14 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -217,7 +479,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -242,9 +504,48 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -257,6 +558,107 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1027" name="AutoShape 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32F41BF4-4670-49DD-9A1F-BDFFABD1E232}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="381000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1028" name="AutoShape 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{768256E8-D99F-4401-A21A-281C812D6C9A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -521,27 +923,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="17.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="11.109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.21875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" style="1" customWidth="1"/>
-    <col min="10" max="39" width="11.109375" style="1" customWidth="1"/>
-    <col min="40" max="40" width="10.77734375" style="1" customWidth="1"/>
-    <col min="41" max="41" width="14.5546875" style="1" customWidth="1"/>
-    <col min="42" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="2" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="11.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" style="1" customWidth="1"/>
+    <col min="10" max="39" width="11.140625" style="1" customWidth="1"/>
+    <col min="40" max="40" width="10.7109375" style="1" customWidth="1"/>
+    <col min="41" max="41" width="14.5703125" style="1" customWidth="1"/>
+    <col min="42" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:41" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -666,11 +1068,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:41" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:41" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="16" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -794,6 +1196,1014 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="vVN9INc/MAVP7T23CbMx/ItHULLViYForWINiN6XR08mGyT6uIptnBC6x9QokMP5VepIf0albxgjxt4c5IXrtA==" saltValue="rlelgKT7zwXxmnutGfptHw==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53099A20-C150-4B8D-B398-C8FF052121BD}">
+  <dimension ref="A1:E91"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="3" max="3" width="79" style="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+    </row>
+    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="20"/>
+      <c r="B6" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="19"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="20"/>
+      <c r="B7" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
+      <c r="B8" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="20"/>
+      <c r="B9" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="19"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="20"/>
+      <c r="B10" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="20"/>
+      <c r="B11" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="19"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="20"/>
+      <c r="B12" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="19"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="20"/>
+      <c r="B13" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="20"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+    </row>
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+      <c r="B18" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="18"/>
+      <c r="B19" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="18"/>
+      <c r="B20" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="19"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="18"/>
+      <c r="B21" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="19"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="18"/>
+      <c r="B22" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="19"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="18"/>
+      <c r="B23" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="19"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="18"/>
+      <c r="B24" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="19"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="18"/>
+      <c r="B25" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="19"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="18"/>
+      <c r="B26" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="19"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="18"/>
+      <c r="B27" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="19"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
+      <c r="B28" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="19"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="18"/>
+      <c r="B29" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="19"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="18"/>
+      <c r="B30" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="19"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="18"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="9"/>
+      <c r="C32" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="20"/>
+      <c r="B33" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="19"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="20"/>
+      <c r="B34" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" s="19"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="20"/>
+      <c r="B35" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" s="19"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="20"/>
+      <c r="B36" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" s="19"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="20"/>
+      <c r="B37" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" s="19"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="20"/>
+      <c r="B38" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" s="19"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="20"/>
+      <c r="B39" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" s="19"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="20"/>
+      <c r="B40" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" s="19"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="20"/>
+      <c r="B41" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="19"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="20"/>
+      <c r="B42" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="19"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="20"/>
+      <c r="B43" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" s="19"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="20"/>
+      <c r="B44" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" s="19"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="20"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+    </row>
+    <row r="46" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+    </row>
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+    </row>
+    <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+    </row>
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+    </row>
+    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C56" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+    </row>
+    <row r="57" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+    </row>
+    <row r="58" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A58" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B59" s="9"/>
+      <c r="C59" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D59" s="17"/>
+      <c r="E59" s="17"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="18"/>
+      <c r="B60" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C60" s="19"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="17"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="18"/>
+      <c r="B61" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C61" s="19"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="17"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="18"/>
+      <c r="B62" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C62" s="19"/>
+      <c r="D62" s="17"/>
+      <c r="E62" s="17"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="18"/>
+      <c r="B63" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C63" s="19"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="17"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="18"/>
+      <c r="B64" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C64" s="19"/>
+      <c r="D64" s="17"/>
+      <c r="E64" s="17"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="18"/>
+      <c r="B65" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C65" s="19"/>
+      <c r="D65" s="17"/>
+      <c r="E65" s="17"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="18"/>
+      <c r="B66" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C66" s="19"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="17"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="18"/>
+      <c r="B67" s="10"/>
+      <c r="C67" s="19"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+    </row>
+    <row r="68" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B68" s="9"/>
+      <c r="C68" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="D68" s="17"/>
+      <c r="E68" s="17"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="18"/>
+      <c r="B69" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C69" s="19"/>
+      <c r="D69" s="17"/>
+      <c r="E69" s="17"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="18"/>
+      <c r="B70" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C70" s="19"/>
+      <c r="D70" s="17"/>
+      <c r="E70" s="17"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="18"/>
+      <c r="B71" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C71" s="19"/>
+      <c r="D71" s="17"/>
+      <c r="E71" s="17"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="18"/>
+      <c r="B72" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C72" s="19"/>
+      <c r="D72" s="17"/>
+      <c r="E72" s="17"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="18"/>
+      <c r="B73" s="10"/>
+      <c r="C73" s="19"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="9"/>
+    </row>
+    <row r="74" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A74" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C74" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
+    </row>
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A75" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C75" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D75" s="9"/>
+      <c r="E75" s="9"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C76" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="D76" s="9"/>
+      <c r="E76" s="9"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B77" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="D77" s="9"/>
+      <c r="E77" s="9"/>
+    </row>
+    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B78" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C78" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C79" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
+    </row>
+    <row r="80" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C80" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D80" s="9"/>
+      <c r="E80" s="9"/>
+    </row>
+    <row r="81" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A81" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B81" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C81" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="D81" s="9"/>
+      <c r="E81" s="9"/>
+    </row>
+    <row r="82" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A82" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C82" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="D82" s="9"/>
+      <c r="E82" s="9"/>
+    </row>
+    <row r="83" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A83" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C83" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D83" s="9"/>
+      <c r="E83" s="9"/>
+    </row>
+    <row r="84" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A84" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C84" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="D84" s="9"/>
+      <c r="E84" s="9"/>
+    </row>
+    <row r="85" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A85" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B85" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C85" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="D85" s="9"/>
+      <c r="E85" s="9"/>
+    </row>
+    <row r="86" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A86" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C86" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D86" s="9"/>
+      <c r="E86" s="9"/>
+    </row>
+    <row r="87" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A87" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C87" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="D87" s="9"/>
+      <c r="E87" s="9"/>
+    </row>
+    <row r="88" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A88" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C88" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D88" s="9"/>
+      <c r="E88" s="9"/>
+    </row>
+    <row r="89" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C89" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D89" s="9"/>
+      <c r="E89" s="9"/>
+    </row>
+    <row r="90" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+      <c r="A90" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B90" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C90" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="D90" s="9"/>
+      <c r="E90" s="9"/>
+    </row>
+    <row r="91" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A91" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C91" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="A5:A14"/>
+    <mergeCell ref="C5:C14"/>
+    <mergeCell ref="D5:D14"/>
+    <mergeCell ref="E5:E14"/>
+    <mergeCell ref="D17:D30"/>
+    <mergeCell ref="E17:E30"/>
+    <mergeCell ref="D68:D72"/>
+    <mergeCell ref="E68:E72"/>
+    <mergeCell ref="A17:A31"/>
+    <mergeCell ref="A59:A67"/>
+    <mergeCell ref="A68:A73"/>
+    <mergeCell ref="C17:C31"/>
+    <mergeCell ref="C68:C73"/>
+    <mergeCell ref="C59:C67"/>
+    <mergeCell ref="A32:A45"/>
+    <mergeCell ref="C32:C45"/>
+    <mergeCell ref="D32:D45"/>
+    <mergeCell ref="E32:E45"/>
+    <mergeCell ref="D59:D66"/>
+    <mergeCell ref="E59:E66"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>